<commit_message>
Added readme text, implemented Fill keyword
</commit_message>
<xml_diff>
--- a/Gears.Interpreter/Scenarios/Test1.xlsx
+++ b/Gears.Interpreter/Scenarios/Test1.xlsx
@@ -16,9 +16,9 @@
   </sheets>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Ondrej Homola - Personal View" guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}" mergeInterval="0" personalView="1" xWindow="270" yWindow="221" windowWidth="1440" windowHeight="759" activeSheetId="1"/>
+    <customWorkbookView name="Petra Homolova – osobní zobrazení" guid="{9EA680E1-9BBC-43CD-B7A0-27FF25AF8532}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
     <customWorkbookView name="user - Personal View" guid="{D7740BFB-74E8-4045-B740-3C7C0F56536C}" mergeInterval="0" personalView="1" xWindow="769" yWindow="185" windowWidth="1151" windowHeight="1000" activeSheetId="1"/>
-    <customWorkbookView name="Petra Homolova – osobní zobrazení" guid="{9EA680E1-9BBC-43CD-B7A0-27FF25AF8532}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Ondrej Homola - Personal View" guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}" mergeInterval="0" personalView="1" xWindow="363" yWindow="161" windowWidth="1440" windowHeight="759" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -52,34 +52,34 @@
     <t>Test Finished</t>
   </si>
   <si>
-    <t>http://www.w3schools.com/</t>
-  </si>
-  <si>
     <t>Click</t>
-  </si>
-  <si>
-    <t>Not Found Text</t>
   </si>
   <si>
     <t>Fill</t>
   </si>
   <si>
-    <t>Search w3schoools.com</t>
-  </si>
-  <si>
-    <t>jquery</t>
-  </si>
-  <si>
     <t>IsTextVisible</t>
-  </si>
-  <si>
-    <t>CSS Example:</t>
   </si>
   <si>
     <t>Expect</t>
   </si>
   <si>
-    <t>Search w3schools</t>
+    <t>http://www.seleniumhq.org/</t>
+  </si>
+  <si>
+    <t>search selenium:</t>
+  </si>
+  <si>
+    <t>download</t>
+  </si>
+  <si>
+    <t>Go</t>
+  </si>
+  <si>
+    <t>Nonexistent Text</t>
+  </si>
+  <si>
+    <t>Selenium IDE</t>
   </si>
 </sst>
 </file>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{11161202-17D5-4CCE-AB10-0CD114CBC98B}" diskRevisions="1" revisionId="93" version="30">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{90DA54A7-BAF4-45FA-8076-A164E778CA5A}" diskRevisions="1" revisionId="121" version="36">
   <header guid="{289ABAFF-1819-46C0-8339-02441CA36636}" dateTime="2016-08-27T21:22:41" maxSheetId="2" userName="Ondrej Homola" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -282,6 +282,36 @@
     </sheetIdMap>
   </header>
   <header guid="{11161202-17D5-4CCE-AB10-0CD114CBC98B}" dateTime="2016-09-04T22:42:08" maxSheetId="2" userName="user" r:id="rId30" minRId="93">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{BA1EAEA7-9888-4997-9F6F-439DC28C08C0}" dateTime="2016-09-05T20:26:09" maxSheetId="2" userName="Ondrej Homola" r:id="rId31" minRId="94" maxRId="112">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{AACEEFB0-3BC2-4B7E-B876-BCB86ED1DEF8}" dateTime="2016-09-05T21:22:44" maxSheetId="2" userName="Ondrej Homola" r:id="rId32" minRId="113">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{AFE8B0A7-28B6-4745-8635-361F913C08C0}" dateTime="2016-09-05T21:27:50" maxSheetId="2" userName="Ondrej Homola" r:id="rId33" minRId="114" maxRId="118">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{2EBDF1E2-CA43-4A83-99DF-57699DBB9D8F}" dateTime="2016-09-05T21:27:55" maxSheetId="2" userName="Ondrej Homola" r:id="rId34" minRId="119">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{0187C503-D90F-461E-86E1-437DA152E359}" dateTime="2016-09-05T21:32:13" maxSheetId="2" userName="Ondrej Homola" r:id="rId35" minRId="120">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{90DA54A7-BAF4-45FA-8076-A164E778CA5A}" dateTime="2016-09-05T21:32:18" maxSheetId="2" userName="Ondrej Homola" r:id="rId36" minRId="121">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -995,6 +1025,256 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog31.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="94" sId="1" xfDxf="1" dxf="1">
+    <oc r="B2" t="inlineStr">
+      <is>
+        <t>http://www.w3schools.com/</t>
+      </is>
+    </oc>
+    <nc r="B2" t="inlineStr">
+      <is>
+        <t>http://www.seleniumhq.org/</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="95" sId="1" ref="A3:XFD3" action="insertRow"/>
+  <rm rId="96" sheetId="1" source="B1:B2" destination="F1:F2" sourceSheetId="1"/>
+  <rrc rId="97" sId="1" ref="B1:B1048576" action="deleteCol">
+    <rfmt sheetId="1" xfDxf="1" sqref="B1:B1048576" start="0" length="0"/>
+  </rrc>
+  <rcc rId="98" sId="1">
+    <nc r="A3" t="inlineStr">
+      <is>
+        <t>Fill</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="99" sId="1">
+    <nc r="B3" t="inlineStr">
+      <is>
+        <t>search selenium:</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="100" sId="1">
+    <nc r="C3" t="inlineStr">
+      <is>
+        <t>download</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="101" sId="1">
+    <oc r="B4" t="inlineStr">
+      <is>
+        <t>Not Found Text</t>
+      </is>
+    </oc>
+    <nc r="B4" t="inlineStr">
+      <is>
+        <t>Go</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="102" sId="1">
+    <oc r="B5" t="inlineStr">
+      <is>
+        <t>Search w3schools</t>
+      </is>
+    </oc>
+    <nc r="B5" t="inlineStr">
+      <is>
+        <t>Download Selenium server</t>
+      </is>
+    </nc>
+  </rcc>
+  <rm rId="103" sheetId="1" source="A5:XFD5" destination="A7:XFD7" sourceSheetId="1">
+    <rfmt sheetId="1" xfDxf="1" sqref="A7:XFD7" start="0" length="0"/>
+    <rcc rId="0" sId="1">
+      <nc r="A7" t="inlineStr">
+        <is>
+          <t>IsTextVisible</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="1">
+      <nc r="C7" t="inlineStr">
+        <is>
+          <t>Search w3schoools.com</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="1">
+      <nc r="D7" t="b">
+        <v>1</v>
+      </nc>
+    </rcc>
+  </rm>
+  <rm rId="104" sheetId="1" source="A6:XFD6" destination="A5:XFD5" sourceSheetId="1">
+    <rfmt sheetId="1" xfDxf="1" sqref="A5:XFD5" start="0" length="0"/>
+  </rm>
+  <rm rId="105" sheetId="1" source="B7" destination="C5" sourceSheetId="1">
+    <rcc rId="0" sId="1">
+      <nc r="C5" t="inlineStr">
+        <is>
+          <t>CSS Example:</t>
+        </is>
+      </nc>
+    </rcc>
+  </rm>
+  <rm rId="106" sheetId="1" source="A7" destination="A6" sourceSheetId="1"/>
+  <rcc rId="107" sId="1">
+    <nc r="B6" t="inlineStr">
+      <is>
+        <t>Download Selenium server</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="108" sId="1" ref="A7:XFD8" action="insertRow"/>
+  <rrc rId="109" sId="1" ref="A7:XFD7" action="deleteRow">
+    <rfmt sheetId="1" xfDxf="1" sqref="A7:XFD7" start="0" length="0"/>
+  </rrc>
+  <rrc rId="110" sId="1" ref="A7:XFD7" action="deleteRow">
+    <rfmt sheetId="1" xfDxf="1" sqref="A7:XFD7" start="0" length="0"/>
+  </rrc>
+  <rrc rId="111" sId="1" ref="A7:XFD7" action="deleteRow">
+    <rfmt sheetId="1" xfDxf="1" sqref="A7:XFD7" start="0" length="0"/>
+  </rrc>
+  <rrc rId="112" sId="1" ref="A7:XFD7" action="deleteRow">
+    <rfmt sheetId="1" xfDxf="1" sqref="A7:XFD7" start="0" length="0"/>
+    <rcc rId="0" sId="1">
+      <nc r="A7" t="inlineStr">
+        <is>
+          <t>Fill</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="1">
+      <nc r="B7" t="inlineStr">
+        <is>
+          <t>Search w3schoools.com</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="1">
+      <nc r="C7" t="inlineStr">
+        <is>
+          <t>jquery</t>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+  <rcv guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}" action="delete"/>
+  <rcv guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog32.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="113" sId="1">
+    <oc r="C5" t="inlineStr">
+      <is>
+        <t>Download Selenium server</t>
+      </is>
+    </oc>
+    <nc r="C5" t="inlineStr">
+      <is>
+        <t>Download Selenium Server</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog33.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="114" sId="1" ref="A6:XFD6" action="insertRow"/>
+  <rcc rId="115" sId="1">
+    <nc r="A6" t="inlineStr">
+      <is>
+        <t>IsTextVisible</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="116" sId="1">
+    <nc r="D6" t="b">
+      <v>1</v>
+    </nc>
+  </rcc>
+  <rcc rId="117" sId="1">
+    <oc r="C5" t="inlineStr">
+      <is>
+        <t>Download Selenium Server</t>
+      </is>
+    </oc>
+    <nc r="C5" t="inlineStr">
+      <is>
+        <t>Selenium Server</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="118" sId="1">
+    <nc r="C6" t="inlineStr">
+      <is>
+        <t>Nonexistent Text</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog34.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="119" sId="1">
+    <oc r="B7" t="inlineStr">
+      <is>
+        <t>Download Selenium server</t>
+      </is>
+    </oc>
+    <nc r="B7" t="inlineStr">
+      <is>
+        <t>Selenium server</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog35.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="120" sId="1">
+    <oc r="C5" t="inlineStr">
+      <is>
+        <t>Selenium Server</t>
+      </is>
+    </oc>
+    <nc r="C5" t="inlineStr">
+      <is>
+        <t>Selenium IDE</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog36.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="121" sId="1">
+    <oc r="B7" t="inlineStr">
+      <is>
+        <t>Selenium server</t>
+      </is>
+    </oc>
+    <nc r="B7" t="inlineStr">
+      <is>
+        <t>Selenium IDE</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rrc rId="5" sId="1" ref="A4:XFD4" action="insertRow"/>
@@ -1149,8 +1429,9 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="2">
   <userInfo guid="{65852624-5F78-4C0A-893F-9FB4020FED43}" name="Ondrej Homola" id="-145669920" dateTime="2016-08-27T21:22:41"/>
+  <userInfo guid="{90DA54A7-BAF4-45FA-8076-A164E778CA5A}" name="Ondrej Homola" id="-145671088" dateTime="2016-09-05T20:19:40"/>
 </users>
 </file>
 
@@ -1454,15 +1735,14 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1470,95 +1750,95 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
+      <c r="E2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="b">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="b">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{D7740BFB-74E8-4045-B740-3C7C0F56536C}">
-      <selection activeCell="D5" sqref="D5"/>
+    <customSheetView guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}">
+      <selection activeCell="A7" sqref="A7:XFD10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{9EA680E1-9BBC-43CD-B7A0-27FF25AF8532}">
       <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}">
-      <selection activeCell="D13" sqref="D13"/>
+    <customSheetView guid="{D7740BFB-74E8-4045-B740-3C7C0F56536C}">
+      <selection activeCell="D5" sqref="D5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
added location-based element search to Fill, added location parameter
</commit_message>
<xml_diff>
--- a/Gears.Interpreter/Scenarios/Test1.xlsx
+++ b/Gears.Interpreter/Scenarios/Test1.xlsx
@@ -16,9 +16,9 @@
   </sheets>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="user - Personal View" guid="{D7740BFB-74E8-4045-B740-3C7C0F56536C}" mergeInterval="0" personalView="1" xWindow="769" yWindow="185" windowWidth="1151" windowHeight="1000" activeSheetId="1"/>
+    <customWorkbookView name="Petra Homolova – osobní zobrazení" guid="{9EA680E1-9BBC-43CD-B7A0-27FF25AF8532}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
     <customWorkbookView name="Ondrej Homola - Personal View" guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}" mergeInterval="0" personalView="1" xWindow="270" yWindow="221" windowWidth="1440" windowHeight="759" activeSheetId="1"/>
-    <customWorkbookView name="Petra Homolova – osobní zobrazení" guid="{9EA680E1-9BBC-43CD-B7A0-27FF25AF8532}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="user - Personal View" guid="{D7740BFB-74E8-4045-B740-3C7C0F56536C}" mergeInterval="0" personalView="1" xWindow="769" yWindow="185" windowWidth="1151" windowHeight="1000" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>GoToUrl</t>
-  </si>
-  <si>
-    <t>Label</t>
   </si>
   <si>
     <t>Text</t>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>Selenium IDE</t>
+  </si>
+  <si>
+    <t>What</t>
   </si>
 </sst>
 </file>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{90DA54A7-BAF4-45FA-8076-A164E778CA5A}" diskRevisions="1" revisionId="121" version="36">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{979FCA90-FA2D-4A6D-9046-745678C05F19}" diskRevisions="1" revisionId="122" version="37">
   <header guid="{289ABAFF-1819-46C0-8339-02441CA36636}" dateTime="2016-08-27T21:22:41" maxSheetId="2" userName="Ondrej Homola" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -312,6 +312,11 @@
     </sheetIdMap>
   </header>
   <header guid="{90DA54A7-BAF4-45FA-8076-A164E778CA5A}" dateTime="2016-09-05T21:32:18" maxSheetId="2" userName="Ondrej Homola" r:id="rId36" minRId="121">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{979FCA90-FA2D-4A6D-9046-745678C05F19}" dateTime="2016-09-09T00:50:10" maxSheetId="2" userName="Ondrej Homola" r:id="rId37" minRId="122">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -1275,6 +1280,23 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog37.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="122" sId="1">
+    <oc r="B1" t="inlineStr">
+      <is>
+        <t>Label</t>
+      </is>
+    </oc>
+    <nc r="B1" t="inlineStr">
+      <is>
+        <t>What</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rrc rId="5" sId="1" ref="A4:XFD4" action="insertRow"/>
@@ -1428,10 +1450,9 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="2">
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
   <userInfo guid="{65852624-5F78-4C0A-893F-9FB4020FED43}" name="Ondrej Homola" id="-145669920" dateTime="2016-08-27T21:22:41"/>
-  <userInfo guid="{90DA54A7-BAF4-45FA-8076-A164E778CA5A}" name="Ondrej Homola" id="-145671088" dateTime="2016-09-05T20:19:40"/>
 </users>
 </file>
 
@@ -1735,7 +1756,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1750,13 +1771,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -1767,34 +1788,34 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -1802,10 +1823,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -1813,32 +1834,32 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
         <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}">
-      <selection activeCell="A7" sqref="A7:XFD10"/>
+    <customSheetView guid="{D7740BFB-74E8-4045-B740-3C7C0F56536C}">
+      <selection activeCell="D5" sqref="D5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{9EA680E1-9BBC-43CD-B7A0-27FF25AF8532}">
       <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{D7740BFB-74E8-4045-B740-3C7C0F56536C}">
-      <selection activeCell="D5" sqref="D5"/>
+    <customSheetView guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}">
+      <selection activeCell="A7" sqref="A7:XFD10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Added distance based sorting
</commit_message>
<xml_diff>
--- a/Gears.Interpreter/Scenarios/Test1.xlsx
+++ b/Gears.Interpreter/Scenarios/Test1.xlsx
@@ -16,9 +16,9 @@
   </sheets>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Ondrej Homola - Personal View" guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}" mergeInterval="0" personalView="1" xWindow="270" yWindow="221" windowWidth="1440" windowHeight="759" activeSheetId="1"/>
     <customWorkbookView name="user - Personal View" guid="{D7740BFB-74E8-4045-B740-3C7C0F56536C}" mergeInterval="0" personalView="1" xWindow="769" yWindow="185" windowWidth="1151" windowHeight="1000" activeSheetId="1"/>
     <customWorkbookView name="Petra Homolova – osobní zobrazení" guid="{9EA680E1-9BBC-43CD-B7A0-27FF25AF8532}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Ondrej Homola - Personal View" guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}" mergeInterval="0" personalView="1" xWindow="270" yWindow="221" windowWidth="1440" windowHeight="759" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Discriminator</t>
   </si>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{979FCA90-FA2D-4A6D-9046-745678C05F19}" diskRevisions="1" revisionId="122" version="37">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{A18D643F-62A4-4854-9FE6-7506D0640798}" diskRevisions="1" revisionId="126" version="39">
   <header guid="{289ABAFF-1819-46C0-8339-02441CA36636}" dateTime="2016-08-27T21:22:41" maxSheetId="2" userName="Ondrej Homola" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -317,6 +317,16 @@
     </sheetIdMap>
   </header>
   <header guid="{979FCA90-FA2D-4A6D-9046-745678C05F19}" dateTime="2016-09-09T00:50:10" maxSheetId="2" userName="Ondrej Homola" r:id="rId37" minRId="122">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{156ABCD5-B9CC-4AA7-B3B2-8D2A9381C48A}" dateTime="2016-09-09T22:08:45" maxSheetId="2" userName="Ondrej Homola" r:id="rId38" minRId="123" maxRId="125">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A18D643F-62A4-4854-9FE6-7506D0640798}" dateTime="2016-09-09T22:10:17" maxSheetId="2" userName="Ondrej Homola" r:id="rId39" minRId="126">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -1297,6 +1307,34 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog38.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="123" sId="1" ref="A4:XFD4" action="insertRow"/>
+  <rcc rId="124" sId="1">
+    <nc r="A4" t="inlineStr">
+      <is>
+        <t>Click</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="125" sId="1">
+    <nc r="B4" t="inlineStr">
+      <is>
+        <t>Go</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog39.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rm rId="126" sheetId="1" source="C6:C7" destination="B6:B7" sourceSheetId="1"/>
+  <rcv guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}" action="delete"/>
+  <rcv guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rrc rId="5" sId="1" ref="A4:XFD4" action="insertRow"/>
@@ -1450,9 +1488,10 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="2">
   <userInfo guid="{65852624-5F78-4C0A-893F-9FB4020FED43}" name="Ondrej Homola" id="-145669920" dateTime="2016-08-27T21:22:41"/>
+  <userInfo guid="{A18D643F-62A4-4854-9FE6-7506D0640798}" name="Ondrej Homola" id="-145677976" dateTime="2016-09-09T22:09:51"/>
 </users>
 </file>
 
@@ -1753,10 +1792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,21 +1851,18 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
+      <c r="B6" t="s">
+        <v>15</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -1834,22 +1870,37 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}">
+      <selection activeCell="B6" sqref="B6:B7"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{D7740BFB-74E8-4045-B740-3C7C0F56536C}">
       <selection activeCell="D5" sqref="D5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1858,10 +1909,6 @@
       <selection activeCell="B9" sqref="B9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}">
-      <selection activeCell="A7" sqref="A7:XFD10"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
#5342 - Redesigned ISerializer, added JUnitSerializer, -junitxml commandline option
</commit_message>
<xml_diff>
--- a/Gears.Interpreter/Scenarios/Test1.xlsx
+++ b/Gears.Interpreter/Scenarios/Test1.xlsx
@@ -136,76 +136,6 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{475606AE-C79C-4113-B4F5-0EF3ECF26CD1}" diskRevisions="1" revisionId="128" version="40">
-  <header guid="{289ABAFF-1819-46C0-8339-02441CA36636}" dateTime="2016-08-27T21:22:41" maxSheetId="2" userName="Ondrej Homola" r:id="rId1">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{DC3E470D-907F-4447-A697-A6E9A2CF559C}" dateTime="2016-08-27T21:40:21" maxSheetId="2" userName="Ondrej Homola" r:id="rId2" minRId="1" maxRId="3">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{74388893-8A5E-4DC7-B03A-8A668EDBBE0C}" dateTime="2016-08-27T21:41:02" maxSheetId="2" userName="Ondrej Homola" r:id="rId3" minRId="4">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{730E409C-2205-444A-8B3E-21A342F82E31}" dateTime="2016-08-27T21:41:39" maxSheetId="2" userName="Ondrej Homola" r:id="rId4" minRId="5" maxRId="8">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{71A9FA4C-7029-49C7-A7A3-6EA465512E8C}" dateTime="2016-08-27T21:42:35" maxSheetId="2" userName="Ondrej Homola" r:id="rId5" minRId="9" maxRId="11">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{C0D2073E-8002-468F-828C-C579C2890280}" dateTime="2016-08-27T21:42:43" maxSheetId="2" userName="Ondrej Homola" r:id="rId6" minRId="12">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{E4417E81-F593-4807-B8E6-96D57ADAA61A}" dateTime="2016-08-27T21:43:52" maxSheetId="2" userName="Ondrej Homola" r:id="rId7" minRId="13">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{5D802366-0E36-45B9-82BF-B52F3232948F}" dateTime="2016-08-27T21:44:24" maxSheetId="2" userName="Ondrej Homola" r:id="rId8" minRId="14">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{1A247225-A3C5-4133-A314-EE10865E0886}" dateTime="2016-08-27T21:45:30" maxSheetId="2" userName="Ondrej Homola" r:id="rId9" minRId="15" maxRId="18">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{0E1E1749-0A55-4A21-AFD6-19EC48E0F877}" dateTime="2016-08-27T21:46:44" maxSheetId="2" userName="Ondrej Homola" r:id="rId10" minRId="19">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{22412E49-7CF4-4208-99D9-87C42A1F5A5D}" dateTime="2016-08-27T22:12:32" maxSheetId="2" userName="Ondrej Homola" r:id="rId11" minRId="20">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{D563C2EB-5B27-46CB-9E4F-676F586E9B28}" dateTime="2016-08-27T22:21:55" maxSheetId="2" userName="Ondrej Homola" r:id="rId12" minRId="21">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{16B15DE3-23FB-4F81-9751-56BD0CE22A47}" dateTime="2016-08-27T22:28:36" maxSheetId="2" userName="Ondrej Homola" r:id="rId13" minRId="22" maxRId="24">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{811535CD-B15E-415E-989D-FAEB7EF08653}" dateTime="2016-08-27T22:29:07" maxSheetId="2" userName="Ondrej Homola" r:id="rId14" minRId="25">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
   <header guid="{65852624-5F78-4C0A-893F-9FB4020FED43}" dateTime="2016-08-27T22:29:42" maxSheetId="2" userName="Ondrej Homola" r:id="rId15" minRId="26">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -337,98 +267,6 @@
     </sheetIdMap>
   </header>
 </headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
-</file>
-
-<file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="19" sId="1">
-    <oc r="D4" t="inlineStr">
-      <is>
-        <t>gn3263827</t>
-      </is>
-    </oc>
-    <nc r="D4"/>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="20" sId="1">
-    <nc r="D4" t="inlineStr">
-      <is>
-        <t>bleble</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="21" sId="1">
-    <oc r="C5" t="inlineStr">
-      <is>
-        <t>Log In</t>
-      </is>
-    </oc>
-    <nc r="C5" t="inlineStr">
-      <is>
-        <t>Log</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog13.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="22" sId="1">
-    <nc r="E1" t="inlineStr">
-      <is>
-        <t>LinkText</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="23" sId="1">
-    <oc r="C5" t="inlineStr">
-      <is>
-        <t>Log</t>
-      </is>
-    </oc>
-    <nc r="C5"/>
-  </rcc>
-  <rcc rId="24" sId="1">
-    <nc r="E5" t="inlineStr">
-      <is>
-        <t>Log In</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="25" sId="1" xfDxf="1" dxf="1">
-    <oc r="B2" t="inlineStr">
-      <is>
-        <t>https://www.facebook.com/</t>
-      </is>
-    </oc>
-    <nc r="B2" t="inlineStr">
-      <is>
-        <t>https://www.facebook.com/login/</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}" action="delete"/>
-  <rcv guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}" action="add"/>
-</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
@@ -760,26 +598,6 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rrc rId="1" sId="1" eol="1" ref="A4:XFD4" action="insertRow"/>
-  <rcc rId="2" sId="1">
-    <nc r="A4" t="inlineStr">
-      <is>
-        <t>Comment</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="3" sId="1">
-    <nc r="D4" t="inlineStr">
-      <is>
-        <t>Test Finished</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
 <file path=xl/revisions/revisionLog20.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="66" sId="1">
@@ -1006,23 +824,6 @@
   <rcc rId="92" sId="1">
     <nc r="E5" t="b">
       <v>1</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="4" sId="1">
-    <oc r="C3" t="inlineStr">
-      <is>
-        <t>E-Mail</t>
-      </is>
-    </oc>
-    <nc r="C3" t="inlineStr">
-      <is>
-        <t>telefon</t>
-      </is>
     </nc>
   </rcc>
 </revisions>
@@ -1340,33 +1141,6 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rrc rId="5" sId="1" ref="A4:XFD4" action="insertRow"/>
-  <rcc rId="6" sId="1">
-    <nc r="A4" t="inlineStr">
-      <is>
-        <t>FillTextField</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="7" sId="1">
-    <nc r="C4" t="inlineStr">
-      <is>
-        <t>Heslo</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="8" sId="1">
-    <nc r="D4" t="inlineStr">
-      <is>
-        <t>gn3263827</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
 <file path=xl/revisions/revisionLog40.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="127" sId="1">
@@ -1390,132 +1164,6 @@
     <nc r="A7" t="inlineStr">
       <is>
         <t>IsVisible</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rrc rId="9" sId="1" ref="A5:XFD5" action="insertRow"/>
-  <rcc rId="10" sId="1">
-    <nc r="A5" t="inlineStr">
-      <is>
-        <t>ClickOn</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="11" sId="1">
-    <nc r="C5" t="inlineStr">
-      <is>
-        <t>Přihlásit</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="12" sId="1">
-    <oc r="C5" t="inlineStr">
-      <is>
-        <t>Přihlásit</t>
-      </is>
-    </oc>
-    <nc r="C5" t="inlineStr">
-      <is>
-        <t>Přihlásit se</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="13" sId="1">
-    <oc r="C5" t="inlineStr">
-      <is>
-        <t>Přihlásit se</t>
-      </is>
-    </oc>
-    <nc r="C5" t="inlineStr">
-      <is>
-        <t>Prihlásit se</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}" action="delete"/>
-  <rcv guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="14" sId="1">
-    <oc r="C5" t="inlineStr">
-      <is>
-        <t>Prihlásit se</t>
-      </is>
-    </oc>
-    <nc r="C5" t="inlineStr">
-      <is>
-        <t>sit se</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="15" sId="1" xfDxf="1" dxf="1">
-    <oc r="B2" t="inlineStr">
-      <is>
-        <t>https://cs-cz.facebook.com/</t>
-      </is>
-    </oc>
-    <nc r="B2" t="inlineStr">
-      <is>
-        <t>https://www.facebook.com/</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="16" sId="1">
-    <oc r="C3" t="inlineStr">
-      <is>
-        <t>telefon</t>
-      </is>
-    </oc>
-    <nc r="C3" t="inlineStr">
-      <is>
-        <t>Email or Phone</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="17" sId="1">
-    <oc r="C4" t="inlineStr">
-      <is>
-        <t>Heslo</t>
-      </is>
-    </oc>
-    <nc r="C4" t="inlineStr">
-      <is>
-        <t>Password</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="18" sId="1">
-    <oc r="C5" t="inlineStr">
-      <is>
-        <t>sit se</t>
-      </is>
-    </oc>
-    <nc r="C5" t="inlineStr">
-      <is>
-        <t>Log In</t>
       </is>
     </nc>
   </rcc>

</xml_diff>

<commit_message>
JUnit output support (#1)
* #5342 - Redesigned ISerializer, added JUnitSerializer, -junitxml commandline option

* DOC screenshots relative path

* DOC screenshots relative path

* #5342 - xunit.bat added comment about junit-viewer installation

* #5342 - xunit.bat renamed to junit.bat
</commit_message>
<xml_diff>
--- a/Gears.Interpreter/Scenarios/Test1.xlsx
+++ b/Gears.Interpreter/Scenarios/Test1.xlsx
@@ -136,76 +136,6 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{475606AE-C79C-4113-B4F5-0EF3ECF26CD1}" diskRevisions="1" revisionId="128" version="40">
-  <header guid="{289ABAFF-1819-46C0-8339-02441CA36636}" dateTime="2016-08-27T21:22:41" maxSheetId="2" userName="Ondrej Homola" r:id="rId1">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{DC3E470D-907F-4447-A697-A6E9A2CF559C}" dateTime="2016-08-27T21:40:21" maxSheetId="2" userName="Ondrej Homola" r:id="rId2" minRId="1" maxRId="3">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{74388893-8A5E-4DC7-B03A-8A668EDBBE0C}" dateTime="2016-08-27T21:41:02" maxSheetId="2" userName="Ondrej Homola" r:id="rId3" minRId="4">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{730E409C-2205-444A-8B3E-21A342F82E31}" dateTime="2016-08-27T21:41:39" maxSheetId="2" userName="Ondrej Homola" r:id="rId4" minRId="5" maxRId="8">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{71A9FA4C-7029-49C7-A7A3-6EA465512E8C}" dateTime="2016-08-27T21:42:35" maxSheetId="2" userName="Ondrej Homola" r:id="rId5" minRId="9" maxRId="11">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{C0D2073E-8002-468F-828C-C579C2890280}" dateTime="2016-08-27T21:42:43" maxSheetId="2" userName="Ondrej Homola" r:id="rId6" minRId="12">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{E4417E81-F593-4807-B8E6-96D57ADAA61A}" dateTime="2016-08-27T21:43:52" maxSheetId="2" userName="Ondrej Homola" r:id="rId7" minRId="13">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{5D802366-0E36-45B9-82BF-B52F3232948F}" dateTime="2016-08-27T21:44:24" maxSheetId="2" userName="Ondrej Homola" r:id="rId8" minRId="14">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{1A247225-A3C5-4133-A314-EE10865E0886}" dateTime="2016-08-27T21:45:30" maxSheetId="2" userName="Ondrej Homola" r:id="rId9" minRId="15" maxRId="18">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{0E1E1749-0A55-4A21-AFD6-19EC48E0F877}" dateTime="2016-08-27T21:46:44" maxSheetId="2" userName="Ondrej Homola" r:id="rId10" minRId="19">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{22412E49-7CF4-4208-99D9-87C42A1F5A5D}" dateTime="2016-08-27T22:12:32" maxSheetId="2" userName="Ondrej Homola" r:id="rId11" minRId="20">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{D563C2EB-5B27-46CB-9E4F-676F586E9B28}" dateTime="2016-08-27T22:21:55" maxSheetId="2" userName="Ondrej Homola" r:id="rId12" minRId="21">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{16B15DE3-23FB-4F81-9751-56BD0CE22A47}" dateTime="2016-08-27T22:28:36" maxSheetId="2" userName="Ondrej Homola" r:id="rId13" minRId="22" maxRId="24">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{811535CD-B15E-415E-989D-FAEB7EF08653}" dateTime="2016-08-27T22:29:07" maxSheetId="2" userName="Ondrej Homola" r:id="rId14" minRId="25">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
   <header guid="{65852624-5F78-4C0A-893F-9FB4020FED43}" dateTime="2016-08-27T22:29:42" maxSheetId="2" userName="Ondrej Homola" r:id="rId15" minRId="26">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -337,98 +267,6 @@
     </sheetIdMap>
   </header>
 </headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
-</file>
-
-<file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="19" sId="1">
-    <oc r="D4" t="inlineStr">
-      <is>
-        <t>gn3263827</t>
-      </is>
-    </oc>
-    <nc r="D4"/>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="20" sId="1">
-    <nc r="D4" t="inlineStr">
-      <is>
-        <t>bleble</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="21" sId="1">
-    <oc r="C5" t="inlineStr">
-      <is>
-        <t>Log In</t>
-      </is>
-    </oc>
-    <nc r="C5" t="inlineStr">
-      <is>
-        <t>Log</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog13.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="22" sId="1">
-    <nc r="E1" t="inlineStr">
-      <is>
-        <t>LinkText</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="23" sId="1">
-    <oc r="C5" t="inlineStr">
-      <is>
-        <t>Log</t>
-      </is>
-    </oc>
-    <nc r="C5"/>
-  </rcc>
-  <rcc rId="24" sId="1">
-    <nc r="E5" t="inlineStr">
-      <is>
-        <t>Log In</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="25" sId="1" xfDxf="1" dxf="1">
-    <oc r="B2" t="inlineStr">
-      <is>
-        <t>https://www.facebook.com/</t>
-      </is>
-    </oc>
-    <nc r="B2" t="inlineStr">
-      <is>
-        <t>https://www.facebook.com/login/</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}" action="delete"/>
-  <rcv guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}" action="add"/>
-</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
@@ -760,26 +598,6 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rrc rId="1" sId="1" eol="1" ref="A4:XFD4" action="insertRow"/>
-  <rcc rId="2" sId="1">
-    <nc r="A4" t="inlineStr">
-      <is>
-        <t>Comment</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="3" sId="1">
-    <nc r="D4" t="inlineStr">
-      <is>
-        <t>Test Finished</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
 <file path=xl/revisions/revisionLog20.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="66" sId="1">
@@ -1006,23 +824,6 @@
   <rcc rId="92" sId="1">
     <nc r="E5" t="b">
       <v>1</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="4" sId="1">
-    <oc r="C3" t="inlineStr">
-      <is>
-        <t>E-Mail</t>
-      </is>
-    </oc>
-    <nc r="C3" t="inlineStr">
-      <is>
-        <t>telefon</t>
-      </is>
     </nc>
   </rcc>
 </revisions>
@@ -1340,33 +1141,6 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rrc rId="5" sId="1" ref="A4:XFD4" action="insertRow"/>
-  <rcc rId="6" sId="1">
-    <nc r="A4" t="inlineStr">
-      <is>
-        <t>FillTextField</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="7" sId="1">
-    <nc r="C4" t="inlineStr">
-      <is>
-        <t>Heslo</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="8" sId="1">
-    <nc r="D4" t="inlineStr">
-      <is>
-        <t>gn3263827</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
 <file path=xl/revisions/revisionLog40.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="127" sId="1">
@@ -1390,132 +1164,6 @@
     <nc r="A7" t="inlineStr">
       <is>
         <t>IsVisible</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rrc rId="9" sId="1" ref="A5:XFD5" action="insertRow"/>
-  <rcc rId="10" sId="1">
-    <nc r="A5" t="inlineStr">
-      <is>
-        <t>ClickOn</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="11" sId="1">
-    <nc r="C5" t="inlineStr">
-      <is>
-        <t>Přihlásit</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="12" sId="1">
-    <oc r="C5" t="inlineStr">
-      <is>
-        <t>Přihlásit</t>
-      </is>
-    </oc>
-    <nc r="C5" t="inlineStr">
-      <is>
-        <t>Přihlásit se</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="13" sId="1">
-    <oc r="C5" t="inlineStr">
-      <is>
-        <t>Přihlásit se</t>
-      </is>
-    </oc>
-    <nc r="C5" t="inlineStr">
-      <is>
-        <t>Prihlásit se</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}" action="delete"/>
-  <rcv guid="{D1C40685-A83F-4D7C-B912-12042843A2EE}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="14" sId="1">
-    <oc r="C5" t="inlineStr">
-      <is>
-        <t>Prihlásit se</t>
-      </is>
-    </oc>
-    <nc r="C5" t="inlineStr">
-      <is>
-        <t>sit se</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="15" sId="1" xfDxf="1" dxf="1">
-    <oc r="B2" t="inlineStr">
-      <is>
-        <t>https://cs-cz.facebook.com/</t>
-      </is>
-    </oc>
-    <nc r="B2" t="inlineStr">
-      <is>
-        <t>https://www.facebook.com/</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="16" sId="1">
-    <oc r="C3" t="inlineStr">
-      <is>
-        <t>telefon</t>
-      </is>
-    </oc>
-    <nc r="C3" t="inlineStr">
-      <is>
-        <t>Email or Phone</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="17" sId="1">
-    <oc r="C4" t="inlineStr">
-      <is>
-        <t>Heslo</t>
-      </is>
-    </oc>
-    <nc r="C4" t="inlineStr">
-      <is>
-        <t>Password</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="18" sId="1">
-    <oc r="C5" t="inlineStr">
-      <is>
-        <t>sit se</t>
-      </is>
-    </oc>
-    <nc r="C5" t="inlineStr">
-      <is>
-        <t>Log In</t>
       </is>
     </nc>
   </rcc>

</xml_diff>